<commit_message>
Now creates the initial setup; notes updated
</commit_message>
<xml_diff>
--- a/doc/ChessBoard.xlsx
+++ b/doc/ChessBoard.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Josue/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Josue/Projects/PlebeianChess/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="157">
   <si>
     <t>0,0</t>
   </si>
@@ -452,10 +452,49 @@
     <t>&lt;&lt;</t>
   </si>
   <si>
-    <t>Logic</t>
-  </si>
-  <si>
-    <t>Visual</t>
+    <t>Notation</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>WP</t>
+  </si>
+  <si>
+    <t>BP</t>
+  </si>
+  <si>
+    <t>WR</t>
+  </si>
+  <si>
+    <t>WN</t>
+  </si>
+  <si>
+    <t>WB</t>
+  </si>
+  <si>
+    <t>WQ</t>
+  </si>
+  <si>
+    <t>WK</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>BQ</t>
+  </si>
+  <si>
+    <t>BK</t>
+  </si>
+  <si>
+    <t>Initial</t>
   </si>
 </sst>
 </file>
@@ -490,7 +529,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -527,11 +566,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -543,6 +604,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -822,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V15"/>
+  <dimension ref="B2:AH15"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA11" sqref="AA11"/>
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.83203125" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -833,15 +909,18 @@
     <col min="1" max="16384" width="4.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>143</v>
+      <c r="AD2" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
-    <row r="3" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O3" s="1">
         <v>97</v>
       </c>
@@ -867,7 +946,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
       <c r="C4" s="3">
         <v>0</v>
@@ -918,8 +997,33 @@
       <c r="V4" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>5</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>6</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4">
         <v>0</v>
       </c>
@@ -944,7 +1048,7 @@
       <c r="I5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N5" s="4">
@@ -971,11 +1075,38 @@
       <c r="U5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="7" t="s">
         <v>93</v>
       </c>
+      <c r="Z5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AH5" s="7" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="6" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4">
         <v>1</v>
       </c>
@@ -1000,7 +1131,7 @@
       <c r="I6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="8" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="4">
@@ -1027,11 +1158,38 @@
       <c r="U6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="8" t="s">
         <v>99</v>
       </c>
+      <c r="Z6" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH6" s="8" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="7" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="4">
         <v>2</v>
       </c>
@@ -1056,7 +1214,7 @@
       <c r="I7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="8" t="s">
         <v>33</v>
       </c>
       <c r="N7" s="4">
@@ -1083,11 +1241,15 @@
       <c r="U7" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="8" t="s">
         <v>110</v>
       </c>
+      <c r="Z7" s="4">
+        <v>2</v>
+      </c>
+      <c r="AH7" s="8"/>
     </row>
-    <row r="8" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4">
         <v>3</v>
       </c>
@@ -1112,7 +1274,7 @@
       <c r="I8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="8" t="s">
         <v>39</v>
       </c>
       <c r="N8" s="4">
@@ -1139,11 +1301,15 @@
       <c r="U8" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="V8" s="8" t="s">
         <v>115</v>
       </c>
+      <c r="Z8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AH8" s="8"/>
     </row>
-    <row r="9" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4">
         <v>4</v>
       </c>
@@ -1168,7 +1334,7 @@
       <c r="I9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="8" t="s">
         <v>45</v>
       </c>
       <c r="N9" s="4">
@@ -1195,11 +1361,15 @@
       <c r="U9" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="V9" s="8" t="s">
         <v>120</v>
       </c>
+      <c r="Z9" s="4">
+        <v>4</v>
+      </c>
+      <c r="AH9" s="8"/>
     </row>
-    <row r="10" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="4">
         <v>5</v>
       </c>
@@ -1224,7 +1394,7 @@
       <c r="I10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="8" t="s">
         <v>51</v>
       </c>
       <c r="N10" s="4">
@@ -1251,11 +1421,15 @@
       <c r="U10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="V10" s="8" t="s">
         <v>125</v>
       </c>
+      <c r="Z10" s="4">
+        <v>5</v>
+      </c>
+      <c r="AH10" s="8"/>
     </row>
-    <row r="11" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="4">
         <v>6</v>
       </c>
@@ -1280,7 +1454,7 @@
       <c r="I11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="8" t="s">
         <v>57</v>
       </c>
       <c r="N11" s="4">
@@ -1307,67 +1481,121 @@
       <c r="U11" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="V11" s="8" t="s">
         <v>130</v>
       </c>
+      <c r="Z11" s="4">
+        <v>6</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AH11" s="8" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="12" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="4">
         <v>7</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="9" t="s">
         <v>63</v>
       </c>
       <c r="N12" s="4">
         <v>1</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="O12" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P12" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="R12" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="S12" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="T12" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="U12" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="V12" s="9" t="s">
         <v>135</v>
       </c>
+      <c r="Z12" s="4">
+        <v>7</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB12" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC12" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD12" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="AE12" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF12" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG12" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH12" s="9" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="14" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F14" s="1" t="s">
         <v>136</v>
       </c>
@@ -1378,7 +1606,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F15" s="1" t="s">
         <v>139</v>
       </c>

</xml_diff>

<commit_message>
Started initial code for moving piece around
</commit_message>
<xml_diff>
--- a/doc/ChessBoard.xlsx
+++ b/doc/ChessBoard.xlsx
@@ -437,9 +437,6 @@
     <t>x,y</t>
   </si>
   <si>
-    <t>(char)(y+97)(x-8)</t>
-  </si>
-  <si>
     <t>ij</t>
   </si>
   <si>
@@ -495,6 +492,9 @@
   </si>
   <si>
     <t>Initial</t>
+  </si>
+  <si>
+    <t>(char)(y+97)(8-x)</t>
   </si>
 </sst>
 </file>
@@ -901,7 +901,7 @@
   <dimension ref="B2:AH15"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.83203125" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -911,13 +911,13 @@
   <sheetData>
     <row r="2" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -1082,28 +1082,28 @@
         <v>0</v>
       </c>
       <c r="AA5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB5" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AC5" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AD5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="AE5" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="AF5" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AH5" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -1165,28 +1165,28 @@
         <v>1</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AH6" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -1488,28 +1488,28 @@
         <v>6</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AF11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AH11" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -1571,28 +1571,28 @@
         <v>7</v>
       </c>
       <c r="AA12" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB12" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="AB12" s="6" t="s">
+      <c r="AC12" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="AC12" s="6" t="s">
+      <c r="AD12" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="AD12" s="6" t="s">
+      <c r="AE12" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="AE12" s="6" t="s">
-        <v>150</v>
-      </c>
       <c r="AF12" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AG12" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AH12" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -1600,21 +1600,21 @@
         <v>136</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F15" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>